<commit_message>
Refactor: move simulator/strategy into invest_adviser.
</commit_message>
<xml_diff>
--- a/input/parameters.xlsx
+++ b/input/parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\MyProject\Python\2021-05-05-crypto-analyzer\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wuyuhao/Projects/Python/20210521-crypto-project/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45AA9C5D-FC4A-4D59-B75A-1C8D15AE1668}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEDF6B8B-45B4-1441-97D4-DEBDAA90D98D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="34245" windowHeight="19965" xr2:uid="{4E6D9016-1A60-43AB-BF93-1824C6880648}"/>
+    <workbookView xWindow="9460" yWindow="2420" windowWidth="34240" windowHeight="19960" xr2:uid="{4E6D9016-1A60-43AB-BF93-1824C6880648}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -466,22 +466,22 @@
   <dimension ref="A1:N94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G87" sqref="G87"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" customWidth="1"/>
+    <col min="8" max="8" width="15.1640625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="13.5" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -510,22 +510,22 @@
         <v>18</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -551,22 +551,22 @@
         <v>19</v>
       </c>
       <c r="I2" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J2">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
+      <c r="M2">
         <v>0.1</v>
       </c>
-      <c r="K2">
+      <c r="N2">
         <v>1.5</v>
       </c>
-      <c r="L2">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -592,22 +592,22 @@
         <v>19</v>
       </c>
       <c r="I3" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J3">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="M3">
         <v>0.2</v>
       </c>
-      <c r="K3">
+      <c r="N3">
         <v>1.6</v>
       </c>
-      <c r="L3">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -633,22 +633,22 @@
         <v>19</v>
       </c>
       <c r="I4" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J4">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="M4">
         <v>0.3</v>
       </c>
-      <c r="K4">
+      <c r="N4">
         <v>1.7</v>
       </c>
-      <c r="L4">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -674,22 +674,22 @@
         <v>19</v>
       </c>
       <c r="I5" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J5">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="M5">
         <v>0.4</v>
       </c>
-      <c r="K5">
+      <c r="N5">
         <v>1.8</v>
       </c>
-      <c r="L5">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -715,22 +715,22 @@
         <v>19</v>
       </c>
       <c r="I6" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J6">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K6">
+        <v>2</v>
+      </c>
+      <c r="M6">
         <v>0.5</v>
       </c>
-      <c r="K6">
+      <c r="N6">
         <v>1.9</v>
       </c>
-      <c r="L6">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -756,22 +756,22 @@
         <v>19</v>
       </c>
       <c r="I7" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J7">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K7">
+        <v>2</v>
+      </c>
+      <c r="M7">
         <v>0.6</v>
       </c>
-      <c r="K7">
-        <v>2</v>
-      </c>
-      <c r="L7">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -797,22 +797,22 @@
         <v>19</v>
       </c>
       <c r="I8" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J8">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K8">
+        <v>2</v>
+      </c>
+      <c r="M8">
         <v>0.7</v>
       </c>
-      <c r="K8">
+      <c r="N8">
         <v>2.1</v>
       </c>
-      <c r="L8">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -838,22 +838,22 @@
         <v>19</v>
       </c>
       <c r="I9" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J9">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K9">
+        <v>2</v>
+      </c>
+      <c r="M9">
         <v>0.8</v>
       </c>
-      <c r="K9">
+      <c r="N9">
         <v>2.2000000000000002</v>
       </c>
-      <c r="L9">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -879,22 +879,22 @@
         <v>19</v>
       </c>
       <c r="I10" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J10">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K10">
+        <v>2</v>
+      </c>
+      <c r="M10">
         <v>0.9</v>
       </c>
-      <c r="K10">
+      <c r="N10">
         <v>2.2999999999999998</v>
       </c>
-      <c r="L10">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -920,22 +920,22 @@
         <v>19</v>
       </c>
       <c r="I11" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J11">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K11">
+        <v>2</v>
+      </c>
+      <c r="M11">
         <v>1</v>
       </c>
-      <c r="K11">
+      <c r="N11">
         <v>2.4</v>
       </c>
-      <c r="L11">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -961,22 +961,22 @@
         <v>19</v>
       </c>
       <c r="I12" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J12">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K12">
+        <v>3</v>
+      </c>
+      <c r="M12">
         <v>0.1</v>
       </c>
-      <c r="K12">
+      <c r="N12">
         <v>1.5</v>
       </c>
-      <c r="L12">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1002,22 +1002,22 @@
         <v>19</v>
       </c>
       <c r="I13" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J13">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K13">
+        <v>3</v>
+      </c>
+      <c r="M13">
         <v>0.2</v>
       </c>
-      <c r="K13">
+      <c r="N13">
         <v>1.6</v>
       </c>
-      <c r="L13">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1043,22 +1043,22 @@
         <v>19</v>
       </c>
       <c r="I14" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J14">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K14">
+        <v>3</v>
+      </c>
+      <c r="M14">
         <v>0.3</v>
       </c>
-      <c r="K14">
+      <c r="N14">
         <v>1.7</v>
       </c>
-      <c r="L14">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1084,22 +1084,22 @@
         <v>19</v>
       </c>
       <c r="I15" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J15">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K15">
+        <v>3</v>
+      </c>
+      <c r="M15">
         <v>0.4</v>
       </c>
-      <c r="K15">
+      <c r="N15">
         <v>1.8</v>
       </c>
-      <c r="L15">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1125,22 +1125,22 @@
         <v>19</v>
       </c>
       <c r="I16" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J16">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K16">
+        <v>3</v>
+      </c>
+      <c r="M16">
         <v>0.5</v>
       </c>
-      <c r="K16">
+      <c r="N16">
         <v>1.9</v>
       </c>
-      <c r="L16">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1166,22 +1166,22 @@
         <v>19</v>
       </c>
       <c r="I17" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J17">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K17">
+        <v>3</v>
+      </c>
+      <c r="M17">
         <v>0.6</v>
       </c>
-      <c r="K17">
-        <v>2</v>
-      </c>
-      <c r="L17">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1207,22 +1207,22 @@
         <v>19</v>
       </c>
       <c r="I18" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J18">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K18">
+        <v>3</v>
+      </c>
+      <c r="M18">
         <v>0.7</v>
       </c>
-      <c r="K18">
+      <c r="N18">
         <v>2.1</v>
       </c>
-      <c r="L18">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1248,22 +1248,22 @@
         <v>19</v>
       </c>
       <c r="I19" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J19">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K19">
+        <v>3</v>
+      </c>
+      <c r="M19">
         <v>0.8</v>
       </c>
-      <c r="K19">
+      <c r="N19">
         <v>2.2000000000000002</v>
       </c>
-      <c r="L19">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1289,22 +1289,22 @@
         <v>19</v>
       </c>
       <c r="I20" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J20">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K20">
+        <v>3</v>
+      </c>
+      <c r="M20">
         <v>0.9</v>
       </c>
-      <c r="K20">
+      <c r="N20">
         <v>2.2999999999999998</v>
       </c>
-      <c r="L20">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M20">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1330,22 +1330,22 @@
         <v>19</v>
       </c>
       <c r="I21" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J21">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K21">
+        <v>3</v>
+      </c>
+      <c r="M21">
         <v>1</v>
       </c>
-      <c r="K21">
+      <c r="N21">
         <v>2.4</v>
       </c>
-      <c r="L21">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M21">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1371,22 +1371,22 @@
         <v>19</v>
       </c>
       <c r="I22" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J22">
+        <v>1E-3</v>
+      </c>
+      <c r="K22">
+        <v>3</v>
+      </c>
+      <c r="M22">
         <v>0.1</v>
       </c>
-      <c r="K22">
+      <c r="N22">
         <v>1.5</v>
       </c>
-      <c r="L22">
-        <v>1E-3</v>
-      </c>
-      <c r="M22">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1412,22 +1412,22 @@
         <v>19</v>
       </c>
       <c r="I23" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J23">
+        <v>1E-3</v>
+      </c>
+      <c r="K23">
+        <v>3</v>
+      </c>
+      <c r="M23">
         <v>0.2</v>
       </c>
-      <c r="K23">
+      <c r="N23">
         <v>1.6</v>
       </c>
-      <c r="L23">
-        <v>1E-3</v>
-      </c>
-      <c r="M23">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1453,22 +1453,22 @@
         <v>19</v>
       </c>
       <c r="I24" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J24">
+        <v>1E-3</v>
+      </c>
+      <c r="K24">
+        <v>3</v>
+      </c>
+      <c r="M24">
         <v>0.3</v>
       </c>
-      <c r="K24">
+      <c r="N24">
         <v>1.7</v>
       </c>
-      <c r="L24">
-        <v>1E-3</v>
-      </c>
-      <c r="M24">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1494,22 +1494,22 @@
         <v>19</v>
       </c>
       <c r="I25" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J25">
+        <v>1E-3</v>
+      </c>
+      <c r="K25">
+        <v>3</v>
+      </c>
+      <c r="M25">
         <v>0.4</v>
       </c>
-      <c r="K25">
+      <c r="N25">
         <v>1.8</v>
       </c>
-      <c r="L25">
-        <v>1E-3</v>
-      </c>
-      <c r="M25">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1535,22 +1535,22 @@
         <v>19</v>
       </c>
       <c r="I26" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J26">
+        <v>1E-3</v>
+      </c>
+      <c r="K26">
+        <v>3</v>
+      </c>
+      <c r="M26">
         <v>0.5</v>
       </c>
-      <c r="K26">
+      <c r="N26">
         <v>1.9</v>
       </c>
-      <c r="L26">
-        <v>1E-3</v>
-      </c>
-      <c r="M26">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1576,22 +1576,22 @@
         <v>19</v>
       </c>
       <c r="I27" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J27">
+        <v>1E-3</v>
+      </c>
+      <c r="K27">
+        <v>3</v>
+      </c>
+      <c r="M27">
         <v>0.6</v>
       </c>
-      <c r="K27">
-        <v>2</v>
-      </c>
-      <c r="L27">
-        <v>1E-3</v>
-      </c>
-      <c r="M27">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1617,22 +1617,22 @@
         <v>19</v>
       </c>
       <c r="I28" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J28">
+        <v>1E-3</v>
+      </c>
+      <c r="K28">
+        <v>3</v>
+      </c>
+      <c r="M28">
         <v>0.7</v>
       </c>
-      <c r="K28">
+      <c r="N28">
         <v>2.1</v>
       </c>
-      <c r="L28">
-        <v>1E-3</v>
-      </c>
-      <c r="M28">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1658,22 +1658,22 @@
         <v>19</v>
       </c>
       <c r="I29" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J29">
+        <v>1E-3</v>
+      </c>
+      <c r="K29">
+        <v>3</v>
+      </c>
+      <c r="M29">
         <v>0.8</v>
       </c>
-      <c r="K29">
+      <c r="N29">
         <v>2.2000000000000002</v>
       </c>
-      <c r="L29">
-        <v>1E-3</v>
-      </c>
-      <c r="M29">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1699,22 +1699,22 @@
         <v>19</v>
       </c>
       <c r="I30" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J30">
+        <v>1E-3</v>
+      </c>
+      <c r="K30">
+        <v>3</v>
+      </c>
+      <c r="M30">
         <v>0.9</v>
       </c>
-      <c r="K30">
+      <c r="N30">
         <v>2.2999999999999998</v>
       </c>
-      <c r="L30">
-        <v>1E-3</v>
-      </c>
-      <c r="M30">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1740,22 +1740,22 @@
         <v>19</v>
       </c>
       <c r="I31" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J31">
+        <v>1E-3</v>
+      </c>
+      <c r="K31">
+        <v>3</v>
+      </c>
+      <c r="M31">
         <v>1</v>
       </c>
-      <c r="K31">
+      <c r="N31">
         <v>2.4</v>
       </c>
-      <c r="L31">
-        <v>1E-3</v>
-      </c>
-      <c r="M31">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1781,22 +1781,22 @@
         <v>19</v>
       </c>
       <c r="I32" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J32">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K32">
+        <v>2</v>
+      </c>
+      <c r="M32">
         <v>0.1</v>
       </c>
-      <c r="K32">
+      <c r="N32">
         <v>1.5</v>
       </c>
-      <c r="L32">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M32">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1822,22 +1822,22 @@
         <v>19</v>
       </c>
       <c r="I33" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J33">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K33">
+        <v>2</v>
+      </c>
+      <c r="M33">
         <v>0.2</v>
       </c>
-      <c r="K33">
+      <c r="N33">
         <v>1.6</v>
       </c>
-      <c r="L33">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M33">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1863,22 +1863,22 @@
         <v>19</v>
       </c>
       <c r="I34" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J34">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K34">
+        <v>2</v>
+      </c>
+      <c r="M34">
         <v>0.3</v>
       </c>
-      <c r="K34">
+      <c r="N34">
         <v>1.7</v>
       </c>
-      <c r="L34">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M34">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1904,22 +1904,22 @@
         <v>19</v>
       </c>
       <c r="I35" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J35">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K35">
+        <v>2</v>
+      </c>
+      <c r="M35">
         <v>0.4</v>
       </c>
-      <c r="K35">
+      <c r="N35">
         <v>1.8</v>
       </c>
-      <c r="L35">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M35">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1945,22 +1945,22 @@
         <v>19</v>
       </c>
       <c r="I36" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J36">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K36">
+        <v>2</v>
+      </c>
+      <c r="M36">
         <v>0.5</v>
       </c>
-      <c r="K36">
+      <c r="N36">
         <v>1.9</v>
       </c>
-      <c r="L36">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1986,22 +1986,22 @@
         <v>19</v>
       </c>
       <c r="I37" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J37">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K37">
+        <v>2</v>
+      </c>
+      <c r="M37">
         <v>0.6</v>
       </c>
-      <c r="K37">
-        <v>2</v>
-      </c>
-      <c r="L37">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M37">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2027,22 +2027,22 @@
         <v>19</v>
       </c>
       <c r="I38" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J38">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K38">
+        <v>2</v>
+      </c>
+      <c r="M38">
         <v>0.7</v>
       </c>
-      <c r="K38">
+      <c r="N38">
         <v>2.1</v>
       </c>
-      <c r="L38">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M38">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2068,22 +2068,22 @@
         <v>19</v>
       </c>
       <c r="I39" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J39">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K39">
+        <v>2</v>
+      </c>
+      <c r="M39">
         <v>0.8</v>
       </c>
-      <c r="K39">
+      <c r="N39">
         <v>2.2000000000000002</v>
       </c>
-      <c r="L39">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M39">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2109,22 +2109,22 @@
         <v>19</v>
       </c>
       <c r="I40" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J40">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K40">
+        <v>2</v>
+      </c>
+      <c r="M40">
         <v>0.9</v>
       </c>
-      <c r="K40">
+      <c r="N40">
         <v>2.2999999999999998</v>
       </c>
-      <c r="L40">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M40">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2150,22 +2150,22 @@
         <v>19</v>
       </c>
       <c r="I41" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J41">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K41">
+        <v>2</v>
+      </c>
+      <c r="M41">
         <v>1</v>
       </c>
-      <c r="K41">
+      <c r="N41">
         <v>2.4</v>
       </c>
-      <c r="L41">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M41">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2191,22 +2191,22 @@
         <v>19</v>
       </c>
       <c r="I42" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J42">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K42">
+        <v>3</v>
+      </c>
+      <c r="M42">
         <v>0.1</v>
       </c>
-      <c r="K42">
+      <c r="N42">
         <v>1.5</v>
       </c>
-      <c r="L42">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M42">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2232,22 +2232,22 @@
         <v>19</v>
       </c>
       <c r="I43" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J43">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K43">
+        <v>3</v>
+      </c>
+      <c r="M43">
         <v>0.2</v>
       </c>
-      <c r="K43">
+      <c r="N43">
         <v>1.6</v>
       </c>
-      <c r="L43">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M43">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2273,22 +2273,22 @@
         <v>19</v>
       </c>
       <c r="I44" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J44">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K44">
+        <v>3</v>
+      </c>
+      <c r="M44">
         <v>0.3</v>
       </c>
-      <c r="K44">
+      <c r="N44">
         <v>1.7</v>
       </c>
-      <c r="L44">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M44">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2314,22 +2314,22 @@
         <v>19</v>
       </c>
       <c r="I45" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J45">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K45">
+        <v>3</v>
+      </c>
+      <c r="M45">
         <v>0.4</v>
       </c>
-      <c r="K45">
+      <c r="N45">
         <v>1.8</v>
       </c>
-      <c r="L45">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M45">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2355,22 +2355,22 @@
         <v>19</v>
       </c>
       <c r="I46" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J46">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K46">
+        <v>3</v>
+      </c>
+      <c r="M46">
         <v>0.5</v>
       </c>
-      <c r="K46">
+      <c r="N46">
         <v>1.9</v>
       </c>
-      <c r="L46">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M46">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2396,22 +2396,22 @@
         <v>19</v>
       </c>
       <c r="I47" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J47">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K47">
+        <v>3</v>
+      </c>
+      <c r="M47">
         <v>0.6</v>
       </c>
-      <c r="K47">
-        <v>2</v>
-      </c>
-      <c r="L47">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M47">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2437,22 +2437,22 @@
         <v>19</v>
       </c>
       <c r="I48" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J48">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K48">
+        <v>3</v>
+      </c>
+      <c r="M48">
         <v>0.7</v>
       </c>
-      <c r="K48">
+      <c r="N48">
         <v>2.1</v>
       </c>
-      <c r="L48">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M48">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2478,22 +2478,22 @@
         <v>19</v>
       </c>
       <c r="I49" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J49">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K49">
+        <v>3</v>
+      </c>
+      <c r="M49">
         <v>0.8</v>
       </c>
-      <c r="K49">
+      <c r="N49">
         <v>2.2000000000000002</v>
       </c>
-      <c r="L49">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M49">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2519,22 +2519,22 @@
         <v>19</v>
       </c>
       <c r="I50" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J50">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K50">
+        <v>3</v>
+      </c>
+      <c r="M50">
         <v>0.9</v>
       </c>
-      <c r="K50">
+      <c r="N50">
         <v>2.2999999999999998</v>
       </c>
-      <c r="L50">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M50">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2560,22 +2560,22 @@
         <v>19</v>
       </c>
       <c r="I51" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J51">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K51">
+        <v>3</v>
+      </c>
+      <c r="M51">
         <v>1</v>
       </c>
-      <c r="K51">
+      <c r="N51">
         <v>2.4</v>
       </c>
-      <c r="L51">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M51">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2601,22 +2601,22 @@
         <v>19</v>
       </c>
       <c r="I52" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J52">
+        <v>1E-3</v>
+      </c>
+      <c r="K52">
+        <v>3</v>
+      </c>
+      <c r="M52">
         <v>0.1</v>
       </c>
-      <c r="K52">
+      <c r="N52">
         <v>1.5</v>
       </c>
-      <c r="L52">
-        <v>1E-3</v>
-      </c>
-      <c r="M52">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2642,22 +2642,22 @@
         <v>19</v>
       </c>
       <c r="I53" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J53">
+        <v>1E-3</v>
+      </c>
+      <c r="K53">
+        <v>3</v>
+      </c>
+      <c r="M53">
         <v>0.2</v>
       </c>
-      <c r="K53">
+      <c r="N53">
         <v>1.6</v>
       </c>
-      <c r="L53">
-        <v>1E-3</v>
-      </c>
-      <c r="M53">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2683,22 +2683,22 @@
         <v>19</v>
       </c>
       <c r="I54" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J54">
+        <v>1E-3</v>
+      </c>
+      <c r="K54">
+        <v>3</v>
+      </c>
+      <c r="M54">
         <v>0.3</v>
       </c>
-      <c r="K54">
+      <c r="N54">
         <v>1.7</v>
       </c>
-      <c r="L54">
-        <v>1E-3</v>
-      </c>
-      <c r="M54">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2724,22 +2724,22 @@
         <v>19</v>
       </c>
       <c r="I55" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J55">
+        <v>1E-3</v>
+      </c>
+      <c r="K55">
+        <v>3</v>
+      </c>
+      <c r="M55">
         <v>0.4</v>
       </c>
-      <c r="K55">
+      <c r="N55">
         <v>1.8</v>
       </c>
-      <c r="L55">
-        <v>1E-3</v>
-      </c>
-      <c r="M55">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2765,22 +2765,22 @@
         <v>19</v>
       </c>
       <c r="I56" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J56">
+        <v>1E-3</v>
+      </c>
+      <c r="K56">
+        <v>3</v>
+      </c>
+      <c r="M56">
         <v>0.5</v>
       </c>
-      <c r="K56">
+      <c r="N56">
         <v>1.9</v>
       </c>
-      <c r="L56">
-        <v>1E-3</v>
-      </c>
-      <c r="M56">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2806,22 +2806,22 @@
         <v>19</v>
       </c>
       <c r="I57" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J57">
+        <v>1E-3</v>
+      </c>
+      <c r="K57">
+        <v>3</v>
+      </c>
+      <c r="M57">
         <v>0.6</v>
       </c>
-      <c r="K57">
-        <v>2</v>
-      </c>
-      <c r="L57">
-        <v>1E-3</v>
-      </c>
-      <c r="M57">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2847,22 +2847,22 @@
         <v>19</v>
       </c>
       <c r="I58" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J58">
+        <v>1E-3</v>
+      </c>
+      <c r="K58">
+        <v>3</v>
+      </c>
+      <c r="M58">
         <v>0.7</v>
       </c>
-      <c r="K58">
+      <c r="N58">
         <v>2.1</v>
       </c>
-      <c r="L58">
-        <v>1E-3</v>
-      </c>
-      <c r="M58">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2888,22 +2888,22 @@
         <v>19</v>
       </c>
       <c r="I59" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J59">
+        <v>1E-3</v>
+      </c>
+      <c r="K59">
+        <v>3</v>
+      </c>
+      <c r="M59">
         <v>0.8</v>
       </c>
-      <c r="K59">
+      <c r="N59">
         <v>2.2000000000000002</v>
       </c>
-      <c r="L59">
-        <v>1E-3</v>
-      </c>
-      <c r="M59">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2929,22 +2929,22 @@
         <v>19</v>
       </c>
       <c r="I60" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J60">
+        <v>1E-3</v>
+      </c>
+      <c r="K60">
+        <v>3</v>
+      </c>
+      <c r="M60">
         <v>0.9</v>
       </c>
-      <c r="K60">
+      <c r="N60">
         <v>2.2999999999999998</v>
       </c>
-      <c r="L60">
-        <v>1E-3</v>
-      </c>
-      <c r="M60">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2970,22 +2970,22 @@
         <v>19</v>
       </c>
       <c r="I61" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J61">
+        <v>1E-3</v>
+      </c>
+      <c r="K61">
+        <v>3</v>
+      </c>
+      <c r="M61">
         <v>1</v>
       </c>
-      <c r="K61">
+      <c r="N61">
         <v>2.4</v>
       </c>
-      <c r="L61">
-        <v>1E-3</v>
-      </c>
-      <c r="M61">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -3011,22 +3011,22 @@
         <v>19</v>
       </c>
       <c r="I62" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J62">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K62">
+        <v>2</v>
+      </c>
+      <c r="M62">
         <v>0.1</v>
       </c>
-      <c r="K62">
+      <c r="N62">
         <v>1.5</v>
       </c>
-      <c r="L62">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M62">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -3052,22 +3052,22 @@
         <v>19</v>
       </c>
       <c r="I63" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J63">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K63">
+        <v>2</v>
+      </c>
+      <c r="M63">
         <v>0.2</v>
       </c>
-      <c r="K63">
+      <c r="N63">
         <v>1.6</v>
       </c>
-      <c r="L63">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M63">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -3093,22 +3093,22 @@
         <v>19</v>
       </c>
       <c r="I64" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J64">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K64">
+        <v>2</v>
+      </c>
+      <c r="M64">
         <v>0.3</v>
       </c>
-      <c r="K64">
+      <c r="N64">
         <v>1.7</v>
       </c>
-      <c r="L64">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M64">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -3134,22 +3134,22 @@
         <v>19</v>
       </c>
       <c r="I65" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J65">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K65">
+        <v>2</v>
+      </c>
+      <c r="M65">
         <v>0.4</v>
       </c>
-      <c r="K65">
+      <c r="N65">
         <v>1.8</v>
       </c>
-      <c r="L65">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M65">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -3175,22 +3175,22 @@
         <v>19</v>
       </c>
       <c r="I66" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J66">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K66">
+        <v>2</v>
+      </c>
+      <c r="M66">
         <v>0.5</v>
       </c>
-      <c r="K66">
+      <c r="N66">
         <v>1.9</v>
       </c>
-      <c r="L66">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M66">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -3216,22 +3216,22 @@
         <v>19</v>
       </c>
       <c r="I67" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J67">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K67">
+        <v>2</v>
+      </c>
+      <c r="M67">
         <v>0.6</v>
       </c>
-      <c r="K67">
-        <v>2</v>
-      </c>
-      <c r="L67">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M67">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -3257,22 +3257,22 @@
         <v>19</v>
       </c>
       <c r="I68" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J68">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K68">
+        <v>2</v>
+      </c>
+      <c r="M68">
         <v>0.7</v>
       </c>
-      <c r="K68">
+      <c r="N68">
         <v>2.1</v>
       </c>
-      <c r="L68">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M68">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
@@ -3298,22 +3298,22 @@
         <v>19</v>
       </c>
       <c r="I69" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J69">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K69">
+        <v>2</v>
+      </c>
+      <c r="M69">
         <v>0.8</v>
       </c>
-      <c r="K69">
+      <c r="N69">
         <v>2.2000000000000002</v>
       </c>
-      <c r="L69">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M69">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -3339,22 +3339,22 @@
         <v>19</v>
       </c>
       <c r="I70" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J70">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K70">
+        <v>2</v>
+      </c>
+      <c r="M70">
         <v>0.9</v>
       </c>
-      <c r="K70">
+      <c r="N70">
         <v>2.2999999999999998</v>
       </c>
-      <c r="L70">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M70">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -3380,22 +3380,22 @@
         <v>19</v>
       </c>
       <c r="I71" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J71">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K71">
+        <v>2</v>
+      </c>
+      <c r="M71">
         <v>1</v>
       </c>
-      <c r="K71">
+      <c r="N71">
         <v>2.4</v>
       </c>
-      <c r="L71">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M71">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
@@ -3421,22 +3421,22 @@
         <v>19</v>
       </c>
       <c r="I72" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J72">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K72">
+        <v>2</v>
+      </c>
+      <c r="M72">
         <v>0.1</v>
       </c>
-      <c r="K72">
+      <c r="N72">
         <v>1.5</v>
       </c>
-      <c r="L72">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M72">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
@@ -3462,22 +3462,22 @@
         <v>19</v>
       </c>
       <c r="I73" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J73">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K73">
+        <v>2</v>
+      </c>
+      <c r="M73">
         <v>0.2</v>
       </c>
-      <c r="K73">
+      <c r="N73">
         <v>1.6</v>
       </c>
-      <c r="L73">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M73">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
@@ -3503,22 +3503,22 @@
         <v>19</v>
       </c>
       <c r="I74" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J74">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K74">
+        <v>2</v>
+      </c>
+      <c r="M74">
         <v>0.3</v>
       </c>
-      <c r="K74">
+      <c r="N74">
         <v>1.7</v>
       </c>
-      <c r="L74">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M74">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
@@ -3544,22 +3544,22 @@
         <v>19</v>
       </c>
       <c r="I75" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J75">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K75">
+        <v>2</v>
+      </c>
+      <c r="M75">
         <v>0.4</v>
       </c>
-      <c r="K75">
+      <c r="N75">
         <v>1.8</v>
       </c>
-      <c r="L75">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M75">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
@@ -3585,22 +3585,22 @@
         <v>19</v>
       </c>
       <c r="I76" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J76">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K76">
+        <v>2</v>
+      </c>
+      <c r="M76">
         <v>0.5</v>
       </c>
-      <c r="K76">
+      <c r="N76">
         <v>1.9</v>
       </c>
-      <c r="L76">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M76">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
@@ -3626,22 +3626,22 @@
         <v>19</v>
       </c>
       <c r="I77" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J77">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K77">
+        <v>2</v>
+      </c>
+      <c r="M77">
         <v>0.6</v>
       </c>
-      <c r="K77">
-        <v>2</v>
-      </c>
-      <c r="L77">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M77">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N77">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
@@ -3667,22 +3667,22 @@
         <v>19</v>
       </c>
       <c r="I78" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J78">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K78">
+        <v>2</v>
+      </c>
+      <c r="M78">
         <v>0.7</v>
       </c>
-      <c r="K78">
+      <c r="N78">
         <v>2.1</v>
       </c>
-      <c r="L78">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M78">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>78</v>
       </c>
@@ -3708,22 +3708,22 @@
         <v>19</v>
       </c>
       <c r="I79" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J79">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K79">
+        <v>2</v>
+      </c>
+      <c r="M79">
         <v>0.8</v>
       </c>
-      <c r="K79">
+      <c r="N79">
         <v>2.2000000000000002</v>
       </c>
-      <c r="L79">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M79">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>79</v>
       </c>
@@ -3749,22 +3749,22 @@
         <v>19</v>
       </c>
       <c r="I80" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J80">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K80">
+        <v>2</v>
+      </c>
+      <c r="M80">
         <v>0.9</v>
       </c>
-      <c r="K80">
+      <c r="N80">
         <v>2.2999999999999998</v>
       </c>
-      <c r="L80">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M80">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>80</v>
       </c>
@@ -3790,22 +3790,22 @@
         <v>19</v>
       </c>
       <c r="I81" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J81">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K81">
+        <v>2</v>
+      </c>
+      <c r="M81">
         <v>1</v>
       </c>
-      <c r="K81">
+      <c r="N81">
         <v>2.4</v>
       </c>
-      <c r="L81">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M81">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>81</v>
       </c>
@@ -3831,22 +3831,22 @@
         <v>19</v>
       </c>
       <c r="I82" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J82">
+        <v>4.4100133020519598E-3</v>
+      </c>
+      <c r="K82">
+        <v>0.94042482754768197</v>
+      </c>
+      <c r="M82">
         <v>-6.12781991416309E-2</v>
       </c>
-      <c r="K82">
+      <c r="N82">
         <v>3.2731140296139101</v>
       </c>
-      <c r="L82">
-        <v>4.4100133020519598E-3</v>
-      </c>
-      <c r="M82">
-        <v>0.94042482754768197</v>
-      </c>
-    </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>82</v>
       </c>
@@ -3872,22 +3872,22 @@
         <v>19</v>
       </c>
       <c r="I83" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J83">
+        <v>3.4255696986459101E-3</v>
+      </c>
+      <c r="K83">
+        <v>3.41461894440372</v>
+      </c>
+      <c r="M83">
         <v>9.7999647483704693E-3</v>
       </c>
-      <c r="K83">
+      <c r="N83">
         <v>0.46292753916427498</v>
       </c>
-      <c r="L83">
-        <v>3.4255696986459101E-3</v>
-      </c>
-      <c r="M83">
-        <v>3.41461894440372</v>
-      </c>
-    </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>83</v>
       </c>
@@ -3913,22 +3913,22 @@
         <v>19</v>
       </c>
       <c r="I84" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J84">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K84">
+        <v>2</v>
+      </c>
+      <c r="M84">
         <v>0.1</v>
       </c>
-      <c r="K84">
+      <c r="N84">
         <v>0.5</v>
       </c>
-      <c r="L84">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M84">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>84</v>
       </c>
@@ -3951,25 +3951,25 @@
         <v>19</v>
       </c>
       <c r="I85" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J85">
+        <v>2.3784997256206101E-3</v>
+      </c>
+      <c r="K85">
+        <v>3.0648528356896501</v>
+      </c>
+      <c r="L85" t="s">
+        <v>12</v>
+      </c>
+      <c r="M85">
         <v>7.1899967358760703E-4</v>
       </c>
-      <c r="K85">
+      <c r="N85">
         <v>0.331736520860619</v>
       </c>
-      <c r="L85">
-        <v>2.3784997256206101E-3</v>
-      </c>
-      <c r="M85">
-        <v>3.0648528356896501</v>
-      </c>
-      <c r="N85" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>85</v>
       </c>
@@ -3992,25 +3992,25 @@
         <v>19</v>
       </c>
       <c r="I86" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J86">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="K86">
+        <v>2</v>
+      </c>
+      <c r="L86" t="s">
+        <v>13</v>
+      </c>
+      <c r="M86">
         <v>0.01</v>
       </c>
-      <c r="K86">
+      <c r="N86">
         <v>0.5</v>
       </c>
-      <c r="L86">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="M86">
-        <v>2</v>
-      </c>
-      <c r="N86" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>86</v>
       </c>
@@ -4033,25 +4033,25 @@
         <v>19</v>
       </c>
       <c r="I87" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J87">
+        <v>3.3881238556444401E-3</v>
+      </c>
+      <c r="K87">
+        <v>0.58523196662204202</v>
+      </c>
+      <c r="L87" t="s">
+        <v>14</v>
+      </c>
+      <c r="M87">
         <v>7.7137627095034397E-2</v>
       </c>
-      <c r="K87">
+      <c r="N87">
         <v>0.147341631456371</v>
       </c>
-      <c r="L87">
-        <v>3.3881238556444401E-3</v>
-      </c>
-      <c r="M87">
-        <v>0.58523196662204202</v>
-      </c>
-      <c r="N87" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>87</v>
       </c>
@@ -4077,22 +4077,22 @@
         <v>19</v>
       </c>
       <c r="I88" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J88">
+        <v>3.3881238556444401E-3</v>
+      </c>
+      <c r="K88">
+        <v>0.58523196662204202</v>
+      </c>
+      <c r="M88">
         <v>7.7137627095034397E-2</v>
       </c>
-      <c r="K88">
+      <c r="N88">
         <v>0.147341631456371</v>
       </c>
-      <c r="L88">
-        <v>3.3881238556444401E-3</v>
-      </c>
-      <c r="M88">
-        <v>0.58523196662204202</v>
-      </c>
-    </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>88</v>
       </c>
@@ -4118,25 +4118,25 @@
         <v>19</v>
       </c>
       <c r="I89" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J89">
+        <v>3.6870000000000002E-3</v>
+      </c>
+      <c r="K89">
+        <v>6.1486150000000004</v>
+      </c>
+      <c r="L89" t="s">
+        <v>15</v>
+      </c>
+      <c r="M89">
         <v>4.8883000000000003E-2</v>
       </c>
-      <c r="K89">
+      <c r="N89">
         <v>0.18237500000000001</v>
       </c>
-      <c r="L89">
-        <v>3.6870000000000002E-3</v>
-      </c>
-      <c r="M89">
-        <v>6.1486150000000004</v>
-      </c>
-      <c r="N89" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>89</v>
       </c>
@@ -4162,22 +4162,22 @@
         <v>19</v>
       </c>
       <c r="I90" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J90">
+        <v>3.6870000000000002E-3</v>
+      </c>
+      <c r="K90">
+        <v>6.1486150000000004</v>
+      </c>
+      <c r="M90">
         <v>4.8883000000000003E-2</v>
       </c>
-      <c r="K90">
+      <c r="N90">
         <v>0.18237500000000001</v>
       </c>
-      <c r="L90">
-        <v>3.6870000000000002E-3</v>
-      </c>
-      <c r="M90">
-        <v>6.1486150000000004</v>
-      </c>
-    </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>90</v>
       </c>
@@ -4203,25 +4203,25 @@
         <v>19</v>
       </c>
       <c r="I91" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J91">
+        <v>3.6110000000000001E-3</v>
+      </c>
+      <c r="K91">
+        <v>2.8670789999999999</v>
+      </c>
+      <c r="L91" t="s">
+        <v>16</v>
+      </c>
+      <c r="M91">
         <v>0.122063</v>
       </c>
-      <c r="K91">
+      <c r="N91">
         <v>0.143455</v>
       </c>
-      <c r="L91">
-        <v>3.6110000000000001E-3</v>
-      </c>
-      <c r="M91">
-        <v>2.8670789999999999</v>
-      </c>
-      <c r="N91" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>91</v>
       </c>
@@ -4247,22 +4247,22 @@
         <v>19</v>
       </c>
       <c r="I92" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J92">
+        <v>3.6110000000000001E-3</v>
+      </c>
+      <c r="K92">
+        <v>2.8670789999999999</v>
+      </c>
+      <c r="M92">
         <v>0.122063</v>
       </c>
-      <c r="K92">
+      <c r="N92">
         <v>0.143455</v>
       </c>
-      <c r="L92">
-        <v>3.6110000000000001E-3</v>
-      </c>
-      <c r="M92">
-        <v>2.8670789999999999</v>
-      </c>
-    </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>92</v>
       </c>
@@ -4288,22 +4288,22 @@
         <v>19</v>
       </c>
       <c r="I93" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J93">
+        <v>8.1560000000000001E-3</v>
+      </c>
+      <c r="K93">
+        <v>0.74069700000000005</v>
+      </c>
+      <c r="M93">
         <v>0.61594599999999999</v>
       </c>
-      <c r="K93">
+      <c r="N93">
         <v>0.99924900000000005</v>
       </c>
-      <c r="L93">
-        <v>8.1560000000000001E-3</v>
-      </c>
-      <c r="M93">
-        <v>0.74069700000000005</v>
-      </c>
-    </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>93</v>
       </c>
@@ -4326,16 +4326,19 @@
         <v>20</v>
       </c>
       <c r="I94" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J94">
+        <v>2.7738933629813798</v>
+      </c>
+      <c r="K94">
+        <v>2</v>
+      </c>
+      <c r="M94">
         <v>6.7664951384996105E-2</v>
       </c>
-      <c r="K94">
+      <c r="N94">
         <v>0.14299286941025699</v>
-      </c>
-      <c r="L94">
-        <v>2.7738933629813798</v>
       </c>
     </row>
   </sheetData>

</xml_diff>